<commit_message>
update test case for konklusi dan lokasi
</commit_message>
<xml_diff>
--- a/docs/TestCase.xlsx
+++ b/docs/TestCase.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\laravel\spk-ahp\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8A00374-B00A-4104-84E7-901CB8F44DF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9F7BE70-0E37-4B12-BE31-FAE9918D3968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{24E59808-9CF7-4FED-9E35-2D71BDE5B406}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="208">
   <si>
     <t>Feature</t>
   </si>
@@ -644,6 +644,161 @@
   </si>
   <si>
     <t>Remove Kategori</t>
+  </si>
+  <si>
+    <t>Konklusi</t>
+  </si>
+  <si>
+    <t>Get Konklusi List</t>
+  </si>
+  <si>
+    <t>Get Konklusi List without Filter</t>
+  </si>
+  <si>
+    <t>Get Konklusi List with Status</t>
+  </si>
+  <si>
+    <t>buka menu manajemen konklusi</t>
+  </si>
+  <si>
+    <t>muncul semua konklusi</t>
+  </si>
+  <si>
+    <t>muncul semua konklusi sesuai dengan status filtered</t>
+  </si>
+  <si>
+    <t>Tambah Konklusi</t>
+  </si>
+  <si>
+    <t>Success Tambah Konklusi</t>
+  </si>
+  <si>
+    <t>http://spk-ahp.test/konklusi/add</t>
+  </si>
+  <si>
+    <t>buka menu konklusi
+tekan tombol Tambah Konklusi
+isi title =&gt; Konklusi Baru
+isi status =&gt; aktif</t>
+  </si>
+  <si>
+    <t>konklusi berhasil ditambah</t>
+  </si>
+  <si>
+    <t>buka menu konklusi
+tekan tombol Tambah konklusi
+isi title =&gt; kosong
+isi status  =&gt; kosong</t>
+  </si>
+  <si>
+    <t>Edit Konklusi</t>
+  </si>
+  <si>
+    <t>Success Edit Konklusi</t>
+  </si>
+  <si>
+    <t>http://spk-ahp.test/konklusi/edit/1</t>
+  </si>
+  <si>
+    <t>buka menu konklusi
+tekan tombol Edit konklusi
+isi title =&gt; konklusi lama
+isi status =&gt; aktif</t>
+  </si>
+  <si>
+    <t>edit konklusi berhasil</t>
+  </si>
+  <si>
+    <t>buka menu konklusi
+tekan tombol Tambah konklusi
+isi title =&gt; kosong
+isi status =&gt; kosong</t>
+  </si>
+  <si>
+    <t>Remove Konklusi</t>
+  </si>
+  <si>
+    <t>Success Remove Konklusi</t>
+  </si>
+  <si>
+    <t>buka menu konklusi
+tekan tombol Delete</t>
+  </si>
+  <si>
+    <t>success hapus konklusi</t>
+  </si>
+  <si>
+    <t>Lokasi</t>
+  </si>
+  <si>
+    <t>Get Lokasi List</t>
+  </si>
+  <si>
+    <t>Get Lokasi List without Filter</t>
+  </si>
+  <si>
+    <t>muncul semua lokasi</t>
+  </si>
+  <si>
+    <t>Get Lokasi List with Status</t>
+  </si>
+  <si>
+    <t>muncul semua lokasi sesuai dengan status filtered</t>
+  </si>
+  <si>
+    <t>Tambah Lokasi</t>
+  </si>
+  <si>
+    <t>Success Tambah Lokasi</t>
+  </si>
+  <si>
+    <t>http://spk-ahp.test/lokasi/add</t>
+  </si>
+  <si>
+    <t>buka menu lokasi
+tekan tombol Tambah lokasi
+isi title =&gt; Lokasi Baru
+isi status =&gt; aktif</t>
+  </si>
+  <si>
+    <t>lokasi berhasil ditambah</t>
+  </si>
+  <si>
+    <t>buka menu lokasi
+tekan tombol Tambah Lokasi
+isi title =&gt; kosong
+isi status  =&gt; kosong</t>
+  </si>
+  <si>
+    <t>Edit Lokasi</t>
+  </si>
+  <si>
+    <t>Success Edit Lokasi</t>
+  </si>
+  <si>
+    <t>http://spk-ahp.test/lokasi/edit/1</t>
+  </si>
+  <si>
+    <t>buka menu lokasi
+tekan tombol Edit lokasi
+isi title =&gt; lokasi lama
+isi status =&gt; aktif</t>
+  </si>
+  <si>
+    <t>edit lokasi berhasil</t>
+  </si>
+  <si>
+    <t>buka menu lokasi
+tekan tombol Tambah Lokasi
+isi title =&gt; kosong
+isi status =&gt; kosong</t>
+  </si>
+  <si>
+    <t>success hapus lokasi</t>
+  </si>
+  <si>
+    <t>buka menu lokasi
+tekan tombol Delete</t>
   </si>
 </sst>
 </file>
@@ -1009,10 +1164,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC3A865B-53D6-4FC7-82C6-D703DBC5F6AF}">
-  <dimension ref="A2:F132"/>
+  <dimension ref="A2:F158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" workbookViewId="0">
-      <selection activeCell="A132" sqref="A132"/>
+    <sheetView tabSelected="1" topLeftCell="A142" workbookViewId="0">
+      <selection activeCell="D160" sqref="D160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2043,11 +2198,11 @@
         <v>78</v>
       </c>
     </row>
-    <row r="129" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D129" s="2"/>
       <c r="E129" s="1"/>
     </row>
-    <row r="130" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
         <v>164</v>
       </c>
@@ -2064,13 +2219,257 @@
         <v>162</v>
       </c>
     </row>
-    <row r="131" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D131" s="2"/>
       <c r="E131" s="1"/>
     </row>
-    <row r="132" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="D132" s="2"/>
-      <c r="E132" s="1"/>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A132" t="s">
+        <v>165</v>
+      </c>
+      <c r="B132" t="s">
+        <v>166</v>
+      </c>
+      <c r="C132" t="s">
+        <v>167</v>
+      </c>
+      <c r="D132" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E132" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F132" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C134" t="s">
+        <v>168</v>
+      </c>
+      <c r="D134" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E134" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F134" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E135" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>172</v>
+      </c>
+      <c r="C136" t="s">
+        <v>173</v>
+      </c>
+      <c r="D136" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E136" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="F136" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C138" t="s">
+        <v>8</v>
+      </c>
+      <c r="D138" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="E138" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="F138" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>178</v>
+      </c>
+      <c r="C140" t="s">
+        <v>179</v>
+      </c>
+      <c r="D140" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E140" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F140" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C142" t="s">
+        <v>8</v>
+      </c>
+      <c r="D142" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E142" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="F142" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D143" s="2"/>
+      <c r="E143" s="1"/>
+    </row>
+    <row r="144" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>184</v>
+      </c>
+      <c r="C144" t="s">
+        <v>185</v>
+      </c>
+      <c r="D144" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E144" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F144" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D145" s="2"/>
+      <c r="E145" s="1"/>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A146" t="s">
+        <v>188</v>
+      </c>
+      <c r="B146" t="s">
+        <v>189</v>
+      </c>
+      <c r="C146" t="s">
+        <v>190</v>
+      </c>
+      <c r="D146" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E146" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F146" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C148" t="s">
+        <v>192</v>
+      </c>
+      <c r="D148" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E148" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F148" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E149" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B150" t="s">
+        <v>194</v>
+      </c>
+      <c r="C150" t="s">
+        <v>195</v>
+      </c>
+      <c r="D150" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E150" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="F150" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C152" t="s">
+        <v>8</v>
+      </c>
+      <c r="D152" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="E152" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="F152" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>200</v>
+      </c>
+      <c r="C154" t="s">
+        <v>201</v>
+      </c>
+      <c r="D154" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E154" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="F154" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="C156" t="s">
+        <v>8</v>
+      </c>
+      <c r="D156" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="E156" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="F156" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D157" s="2"/>
+      <c r="E157" s="1"/>
+    </row>
+    <row r="158" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B158" t="s">
+        <v>184</v>
+      </c>
+      <c r="C158" t="s">
+        <v>185</v>
+      </c>
+      <c r="D158" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E158" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="F158" t="s">
+        <v>206</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -2101,6 +2500,20 @@
     <hyperlink ref="D122" r:id="rId25" xr:uid="{068BE442-6A9E-4B8B-A05D-B002822F86D7}"/>
     <hyperlink ref="D124" r:id="rId26" xr:uid="{0F4E77ED-1FE7-4DE9-A954-0FE0A0FA3A95}"/>
     <hyperlink ref="D128" r:id="rId27" xr:uid="{8100857A-5688-49C6-8BA9-8A4A77523B23}"/>
+    <hyperlink ref="D140" r:id="rId28" xr:uid="{6B67C99F-E53E-4D23-B64F-C576CC2C5430}"/>
+    <hyperlink ref="D144" r:id="rId29" xr:uid="{290D09DF-923D-4AE3-B8E5-81002C6DE83D}"/>
+    <hyperlink ref="D142" r:id="rId30" xr:uid="{41F09BE1-24F7-44DE-A97D-8EE66030977F}"/>
+    <hyperlink ref="D132" r:id="rId31" xr:uid="{DBE94C37-B286-4B07-B7C2-636435B68238}"/>
+    <hyperlink ref="D134" r:id="rId32" xr:uid="{E64A0377-2D65-498D-82D0-97E5836A3669}"/>
+    <hyperlink ref="D136" r:id="rId33" xr:uid="{613D05DC-85C3-4918-BF74-C69AD515922A}"/>
+    <hyperlink ref="D138" r:id="rId34" xr:uid="{1068BA93-156F-4ED4-8C67-865962166B63}"/>
+    <hyperlink ref="D154" r:id="rId35" xr:uid="{77DB95E3-DA23-4A9F-9B86-DFDDCC793D09}"/>
+    <hyperlink ref="D158" r:id="rId36" xr:uid="{CD4E4C7D-FF2A-4730-8FDB-416C0F47E37C}"/>
+    <hyperlink ref="D156" r:id="rId37" xr:uid="{0528656E-B0D7-4149-89D8-825A345F0DCF}"/>
+    <hyperlink ref="D146" r:id="rId38" xr:uid="{8FD1DA30-699F-4512-A2AD-7ACB74A5BF5A}"/>
+    <hyperlink ref="D148" r:id="rId39" xr:uid="{25AF89E0-7BDF-4422-803B-41A4FCBAC467}"/>
+    <hyperlink ref="D150" r:id="rId40" xr:uid="{4E7E3015-30A3-4AD9-96CA-764A929D0B61}"/>
+    <hyperlink ref="D152" r:id="rId41" xr:uid="{638D1552-FB26-4E61-A4F4-C38A316BBAF4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>